<commit_message>
Modificar asignacion de colores en las observaciones
</commit_message>
<xml_diff>
--- a/servidor/plantillasRegistro/plantillaGeneral.xlsx
+++ b/servidor/plantillasRegistro/plantillaGeneral.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9254FBA-0459-DD4B-B893-94019ACF0D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D987A954-DE9D-CE46-BDB4-EE574FE85FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{3A45B0B0-08CA-42E0-9056-E9A55D404734}"/>
+    <workbookView xWindow="33380" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{3A45B0B0-08CA-42E0-9056-E9A55D404734}"/>
   </bookViews>
   <sheets>
     <sheet name="Horario" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>DESCRIPCION</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>HORARIO_NOCTURNO</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -464,49 +467,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B07B46C-A95A-46D9-8A69-EA2909F7D79B}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="A2:F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{992F6D4C-7109-4DA7-B3E7-C4A3D7A32869}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{992F6D4C-7109-4DA7-B3E7-C4A3D7A32869}">
       <formula1>"Si,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{8916F1CF-B8B2-44DC-AF72-DF70D8201925}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{8916F1CF-B8B2-44DC-AF72-DF70D8201925}">
       <formula1>"Laborable,Libre,Feriado"</formula1>
     </dataValidation>
   </dataValidations>
@@ -516,79 +523,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD02BAB4-71ED-4E34-B15A-2E3A9D95EADC}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C6" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C14" s="3"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D14" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{41FF5BA2-947E-4F2B-A824-4B008FD67627}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{41FF5BA2-947E-4F2B-A824-4B008FD67627}">
       <formula1>"Entrada,Inicio alimentación,Fin alimentación,Salida"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{D362D15A-CF93-4355-AF96-C60118735F72}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{D362D15A-CF93-4355-AF96-C60118735F72}">
       <formula1>"Si,No"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F1048576" xr:uid="{EC1D5E67-183D-44E4-B8A0-EE08BDF8385A}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G1048576" xr:uid="{EC1D5E67-183D-44E4-B8A0-EE08BDF8385A}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>